<commit_message>
Fixed invoice and label filter, and applied validation.
</commit_message>
<xml_diff>
--- a/public/template/Invoice-Template.xlsx
+++ b/public/template/Invoice-Template.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <si>
     <t>INVOICE NO</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>SKU</t>
+  </si>
+  <si>
+    <t>BAG NO.</t>
   </si>
 </sst>
 </file>
@@ -148,12 +151,17 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -204,7 +212,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -218,6 +226,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="4" applyFont="1" fillId="2" applyFill="1" borderId="0" applyBorder="1" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -535,11 +544,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="AB1" sqref="AB1"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
+      <selection activeCell="AB6" sqref="AB6" activeCellId="0"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="18.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
@@ -569,7 +578,7 @@
     <col min="27" max="27" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" customFormat="1" s="10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -651,8 +660,11 @@
       <c r="AA1" s="9" t="s">
         <v>24</v>
       </c>
+      <c r="AB1" s="11" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="2">
       <c r="A2" s="5"/>
       <c r="B2" s="6"/>
       <c r="F2" s="5"/>
@@ -678,7 +690,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -690,7 +702,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
order details save into invoice table
</commit_message>
<xml_diff>
--- a/public/template/Invoice-Template.xlsx
+++ b/public/template/Invoice-Template.xlsx
@@ -1,28 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\laragon\www\mg3h-sp-api\public\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\laragon\www\amazon-sp-api-laravel\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39BD1B49-8209-43F1-9720-29E1CD5ED8B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>INVOICE NO</t>
   </si>
@@ -106,16 +105,16 @@
   </si>
   <si>
     <t>BAG NO.</t>
+  </si>
+  <si>
+    <t>AMAZON ORDER IDENTIFIER</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,19 +129,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,7 +137,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -161,6 +147,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -208,11 +200,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -220,16 +211,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="4" applyFont="1" fillId="2" applyFill="1" borderId="0" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -541,44 +532,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AC122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
-      <selection activeCell="AB6" sqref="AB6" activeCellId="0"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.54296875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.81640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="4.44140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.453125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="15" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="24.54296875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.453125" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="17" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="24.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="1" s="10">
+    <row r="1" spans="1:29" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -645,38 +637,404 @@
       <c r="V1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="9" t="s">
+      <c r="W1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="9" t="s">
+      <c r="X1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" s="9" t="s">
+      <c r="Y1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" s="9" t="s">
+      <c r="Z1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" s="9" t="s">
+      <c r="AA1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="AB1" s="11" t="s">
+      <c r="AB1" s="8" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="5"/>
-      <c r="B2" s="6"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="8"/>
-      <c r="P2" s="7"/>
-      <c r="T2" s="7"/>
+      <c r="AC1" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="B2" s="5"/>
+      <c r="I2" s="9"/>
+      <c r="K2" s="9"/>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="B3" s="5"/>
+      <c r="I3" s="9"/>
+      <c r="K3" s="9"/>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="B4" s="5"/>
+      <c r="I4" s="9"/>
+      <c r="K4" s="9"/>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="B5" s="5"/>
+      <c r="I5" s="9"/>
+      <c r="K5" s="9"/>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="B6" s="5"/>
+      <c r="I6" s="9"/>
+      <c r="K6" s="9"/>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="B7" s="5"/>
+      <c r="I7" s="9"/>
+      <c r="K7" s="9"/>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="B8" s="5"/>
+      <c r="I8" s="9"/>
+      <c r="K8" s="9"/>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="B9" s="5"/>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="B10" s="5"/>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="B11" s="5"/>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="B12" s="5"/>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="B13" s="5"/>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="B14" s="5"/>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="B15" s="5"/>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="B16" s="5"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B17" s="5"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B18" s="5"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B19" s="5"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B20" s="5"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B21" s="5"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B22" s="5"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B23" s="5"/>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B24" s="5"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B25" s="5"/>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B26" s="5"/>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B27" s="5"/>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B28" s="5"/>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B29" s="5"/>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B30" s="5"/>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B31" s="5"/>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B32" s="5"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B33" s="5"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B34" s="5"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B35" s="5"/>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B36" s="5"/>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B37" s="5"/>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B38" s="5"/>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B39" s="5"/>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B40" s="5"/>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B41" s="5"/>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B42" s="5"/>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B43" s="5"/>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B44" s="5"/>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B45" s="5"/>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B46" s="5"/>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B47" s="5"/>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B48" s="5"/>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B49" s="5"/>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B50" s="5"/>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B51" s="5"/>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B52" s="5"/>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B53" s="5"/>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B54" s="5"/>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B55" s="5"/>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B56" s="5"/>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B57" s="5"/>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B58" s="5"/>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B59" s="5"/>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B60" s="5"/>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B61" s="5"/>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B62" s="5"/>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B63" s="5"/>
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B64" s="5"/>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B65" s="5"/>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B66" s="5"/>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B67" s="5"/>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B68" s="5"/>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B69" s="5"/>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B70" s="5"/>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B71" s="5"/>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B72" s="5"/>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B73" s="5"/>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B74" s="5"/>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B75" s="5"/>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B76" s="5"/>
+    </row>
+    <row r="77" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B77" s="5"/>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B78" s="5"/>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B79" s="5"/>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B80" s="5"/>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B81" s="5"/>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B82" s="5"/>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B83" s="5"/>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B84" s="5"/>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B85" s="5"/>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B86" s="5"/>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B87" s="5"/>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B88" s="5"/>
+    </row>
+    <row r="89" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B89" s="5"/>
+    </row>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B90" s="5"/>
+    </row>
+    <row r="91" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B91" s="5"/>
+    </row>
+    <row r="92" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B92" s="5"/>
+    </row>
+    <row r="93" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B93" s="5"/>
+    </row>
+    <row r="94" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B94" s="5"/>
+    </row>
+    <row r="95" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B95" s="5"/>
+    </row>
+    <row r="96" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B96" s="5"/>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B97" s="5"/>
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B98" s="5"/>
+    </row>
+    <row r="99" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B99" s="5"/>
+    </row>
+    <row r="100" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B100" s="5"/>
+    </row>
+    <row r="101" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B101" s="5"/>
+    </row>
+    <row r="102" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B102" s="5"/>
+    </row>
+    <row r="103" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B103" s="5"/>
+    </row>
+    <row r="104" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B104" s="5"/>
+    </row>
+    <row r="105" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B105" s="5"/>
+    </row>
+    <row r="106" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B106" s="5"/>
+    </row>
+    <row r="107" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B107" s="5"/>
+    </row>
+    <row r="108" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B108" s="5"/>
+    </row>
+    <row r="109" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B109" s="5"/>
+    </row>
+    <row r="110" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B110" s="5"/>
+    </row>
+    <row r="111" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B111" s="5"/>
+    </row>
+    <row r="112" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B112" s="5"/>
+    </row>
+    <row r="113" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B113" s="5"/>
+    </row>
+    <row r="114" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B114" s="5"/>
+    </row>
+    <row r="115" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B115" s="5"/>
+    </row>
+    <row r="116" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B116" s="5"/>
+    </row>
+    <row r="117" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B117" s="5"/>
+    </row>
+    <row r="118" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B118" s="5"/>
+    </row>
+    <row r="119" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B119" s="5"/>
+    </row>
+    <row r="120" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B120" s="5"/>
+    </row>
+    <row r="121" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B121" s="5"/>
+    </row>
+    <row r="122" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B122" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -685,24 +1043,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>